<commit_message>
New style and authorizing
</commit_message>
<xml_diff>
--- a/WebApplication1/Книга1.xlsx
+++ b/WebApplication1/Книга1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Фабрика</t>
   </si>
@@ -41,19 +41,34 @@
     <t>Тп сміття2</t>
   </si>
   <si>
-    <t>Котигорошко</t>
-  </si>
-  <si>
     <t>http://www.kotygoroshko.com.ua</t>
   </si>
   <si>
     <t>м. Львів</t>
   </si>
   <si>
-    <t>Пластмаси</t>
-  </si>
-  <si>
     <t>Папір</t>
+  </si>
+  <si>
+    <t>Пластмаси3333</t>
+  </si>
+  <si>
+    <t>Волт</t>
+  </si>
+  <si>
+    <t>http://www.wolt.com.ua</t>
+  </si>
+  <si>
+    <t>Акамулятор</t>
+  </si>
+  <si>
+    <t>Акація234</t>
+  </si>
+  <si>
+    <t>http://www.aka/ua</t>
+  </si>
+  <si>
+    <t>м. Чернігів</t>
   </si>
 </sst>
 </file>
@@ -384,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,25 +425,52 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>9999</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>